<commit_message>
LLM types testing and I create a table for results
Gemini 2.5 pro
Gemini 1.5 pro
Gemini 2.5 Flash
</commit_message>
<xml_diff>
--- a/LLMTypeTesting/LLM_types_avarage_table.xlsx
+++ b/LLMTypeTesting/LLM_types_avarage_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\LLMTypeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57FEC451-39AD-486B-8E89-7B255D703DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74403DDB-CDE0-4E39-A950-BF867C017A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5144DE4C-A411-45F3-B410-1308A058895F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>LLM modell neve</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>10.57/s</t>
+  </si>
+  <si>
+    <t>gemini-2.5-pro-preview-05-06</t>
+  </si>
+  <si>
+    <t>11.47/s</t>
+  </si>
+  <si>
+    <t>gemini-1.5-pro</t>
+  </si>
+  <si>
+    <t>9.82/s</t>
+  </si>
+  <si>
+    <t>gemini-2.5-flash-preview-04-17</t>
+  </si>
+  <si>
+    <t>10.12/s</t>
   </si>
 </sst>
 </file>
@@ -510,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B60AA78-0292-4A9F-9659-C21A27D67000}">
-  <dimension ref="B3:F10"/>
+  <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,13 +610,13 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6">
         <v>0.84</v>
       </c>
     </row>
@@ -611,6 +629,39 @@
       </c>
       <c r="D10" s="4">
         <v>0.82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I create table for use LLM model information and correcting column names
</commit_message>
<xml_diff>
--- a/LLMTypeTesting/LLM_types_avarage_table.xlsx
+++ b/LLMTypeTesting/LLM_types_avarage_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\LLMTypeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74403DDB-CDE0-4E39-A950-BF867C017A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C3332-1F1C-4DC2-A869-E9907DAFF5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5144DE4C-A411-45F3-B410-1308A058895F}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add new column: Estimated cost of 20 questions
</commit_message>
<xml_diff>
--- a/LLMTypeTesting/LLM_types_avarage_table.xlsx
+++ b/LLMTypeTesting/LLM_types_avarage_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\LLMTypeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C3332-1F1C-4DC2-A869-E9907DAFF5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C7DF76-9749-4F36-8C1A-4AFAE356B733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5144DE4C-A411-45F3-B410-1308A058895F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>LLM modell neve</t>
   </si>
@@ -105,12 +105,21 @@
   </si>
   <si>
     <t>10.12/s</t>
+  </si>
+  <si>
+    <t>Költség becslés 20 kérdésre</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +201,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -531,14 +543,14 @@
   <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="4" max="5" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
@@ -551,7 +563,9 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -564,6 +578,9 @@
       <c r="D4" s="4">
         <v>0.79</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -575,6 +592,9 @@
       <c r="D5" s="4">
         <v>0.78</v>
       </c>
+      <c r="E5" s="7">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -586,6 +606,9 @@
       <c r="D6" s="4">
         <v>0.83</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
@@ -597,6 +620,9 @@
       <c r="D7" s="6">
         <v>0.86</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
@@ -608,6 +634,9 @@
       <c r="D8" s="4">
         <v>0.82</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
@@ -619,6 +648,9 @@
       <c r="D9" s="6">
         <v>0.84</v>
       </c>
+      <c r="E9" s="7">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
@@ -630,6 +662,9 @@
       <c r="D10" s="4">
         <v>0.82</v>
       </c>
+      <c r="E10" s="7">
+        <v>1.29</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
@@ -641,6 +676,9 @@
       <c r="D11" s="6">
         <v>0.85</v>
       </c>
+      <c r="E11" s="7">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
@@ -652,6 +690,9 @@
       <c r="D12" s="4">
         <v>0.8</v>
       </c>
+      <c r="E12" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
@@ -662,6 +703,9 @@
       </c>
       <c r="D13" s="4">
         <v>0.83</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>